<commit_message>
Cleaned Up Analysis, Added Summary Pics
</commit_message>
<xml_diff>
--- a/RawData/StateReopening/FinalData.xlsx
+++ b/RawData/StateReopening/FinalData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ron\StanfordCoronavirusResearch\RawData\StateReopening\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E3DEB44-4975-4205-B393-01907575B0C8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05AB1F6A-10EB-4E35-834A-59562A69B865}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="24000" windowHeight="10170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -91,9 +91,6 @@
     <t>Florida</t>
   </si>
   <si>
-    <t>0605 0627</t>
-  </si>
-  <si>
     <t>0512 0626 0627</t>
   </si>
   <si>
@@ -353,6 +350,9 @@
   </si>
   <si>
     <t>Full Retail</t>
+  </si>
+  <si>
+    <t>0606 0627</t>
   </si>
 </sst>
 </file>
@@ -622,7 +622,7 @@
   <dimension ref="A1:O52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -637,46 +637,46 @@
     <row r="1" spans="1:15" ht="38.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="F1" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="L1" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="K1" s="2" t="s">
-        <v>109</v>
-      </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>106</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>107</v>
       </c>
       <c r="N1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
@@ -1020,7 +1020,7 @@
       </c>
       <c r="B11" s="1"/>
       <c r="C11" s="1" t="s">
-        <v>23</v>
+        <v>110</v>
       </c>
       <c r="D11" s="3">
         <v>504</v>
@@ -1031,7 +1031,7 @@
       </c>
       <c r="G11" s="1"/>
       <c r="H11" s="3">
-        <v>605</v>
+        <v>607</v>
       </c>
       <c r="I11" s="3">
         <v>518</v>
@@ -1040,7 +1040,7 @@
         <v>605</v>
       </c>
       <c r="K11" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="L11" s="1"/>
       <c r="M11" s="1"/>
@@ -1051,7 +1051,7 @@
     </row>
     <row r="12" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="3">
@@ -1084,7 +1084,7 @@
     </row>
     <row r="13" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B13" s="1"/>
       <c r="C13" s="3">
@@ -1127,7 +1127,7 @@
     </row>
     <row r="14" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B14" s="1"/>
       <c r="C14" s="3">
@@ -1160,17 +1160,17 @@
     </row>
     <row r="15" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>29</v>
       </c>
       <c r="C15" s="1"/>
       <c r="D15" s="3">
         <v>626</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F15" s="3">
         <v>529</v>
@@ -1201,7 +1201,7 @@
     </row>
     <row r="16" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B16" s="1"/>
       <c r="C16" s="3">
@@ -1240,7 +1240,7 @@
     </row>
     <row r="17" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B17" s="1"/>
       <c r="C17" s="3">
@@ -1277,7 +1277,7 @@
     </row>
     <row r="18" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B18" s="1"/>
       <c r="C18" s="3">
@@ -1314,11 +1314,11 @@
     </row>
     <row r="19" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1"/>
       <c r="C19" s="1" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3">
         <v>522</v>
@@ -1355,19 +1355,19 @@
     </row>
     <row r="20" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="C20" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>38</v>
       </c>
       <c r="D20" s="3">
         <v>515</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F20" s="3">
         <v>515</v>
@@ -1396,7 +1396,7 @@
     </row>
     <row r="21" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B21" s="1"/>
       <c r="C21" s="3">
@@ -1433,10 +1433,10 @@
     </row>
     <row r="22" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="C22" s="3">
         <v>709</v>
@@ -1478,10 +1478,10 @@
     </row>
     <row r="23" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>42</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>43</v>
       </c>
       <c r="C23" s="1"/>
       <c r="D23" s="3">
@@ -1519,7 +1519,7 @@
     </row>
     <row r="24" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B24" s="1"/>
       <c r="C24" s="3">
@@ -1529,7 +1529,7 @@
         <v>522</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F24" s="3">
         <v>522</v>
@@ -1560,7 +1560,7 @@
     </row>
     <row r="25" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B25" s="1"/>
       <c r="C25" s="3">
@@ -1568,7 +1568,7 @@
       </c>
       <c r="D25" s="1"/>
       <c r="E25" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F25" s="3">
         <v>518</v>
@@ -1599,7 +1599,7 @@
     </row>
     <row r="26" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B26" s="1"/>
       <c r="C26" s="3">
@@ -1636,7 +1636,7 @@
     </row>
     <row r="27" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -1671,7 +1671,7 @@
     </row>
     <row r="28" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B28" s="1"/>
       <c r="C28" s="3">
@@ -1706,7 +1706,7 @@
     </row>
     <row r="29" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B29" s="1"/>
       <c r="C29" s="3">
@@ -1741,7 +1741,7 @@
     </row>
     <row r="30" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B30" s="1"/>
       <c r="C30" s="3">
@@ -1751,7 +1751,7 @@
         <v>509</v>
       </c>
       <c r="E30" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="F30" s="3">
         <v>509</v>
@@ -1780,10 +1780,10 @@
     </row>
     <row r="31" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B31" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="B31" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="C31" s="1"/>
       <c r="D31" s="3">
@@ -1806,7 +1806,7 @@
         <v>615</v>
       </c>
       <c r="K31" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L31" s="1"/>
       <c r="M31" s="1"/>
@@ -1817,7 +1817,7 @@
     </row>
     <row r="32" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B32" s="3">
         <v>615</v>
@@ -1825,7 +1825,7 @@
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F32" s="3">
         <v>615</v>
@@ -1853,22 +1853,22 @@
         <v>522</v>
       </c>
       <c r="O32" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="33" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B33" s="1" t="s">
-        <v>61</v>
       </c>
       <c r="C33" s="1"/>
       <c r="D33" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="E33" s="1" t="s">
         <v>62</v>
-      </c>
-      <c r="E33" s="1" t="s">
-        <v>63</v>
       </c>
       <c r="F33" s="3">
         <v>516</v>
@@ -1897,7 +1897,7 @@
     </row>
     <row r="34" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B34" s="3">
         <v>604</v>
@@ -1907,7 +1907,7 @@
         <v>612</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="F34" s="3">
         <v>530</v>
@@ -1938,7 +1938,7 @@
     </row>
     <row r="35" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -1967,7 +1967,7 @@
     </row>
     <row r="36" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B36" s="1"/>
       <c r="C36" s="3">
@@ -2000,10 +2000,10 @@
     </row>
     <row r="37" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="B37" s="1" t="s">
-        <v>69</v>
       </c>
       <c r="C37" s="3">
         <v>521</v>
@@ -2039,7 +2039,7 @@
     </row>
     <row r="38" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B38" s="1"/>
       <c r="C38" s="3">
@@ -2059,7 +2059,7 @@
         <v>501</v>
       </c>
       <c r="I38" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="J38" s="3">
         <v>501</v>
@@ -2078,14 +2078,14 @@
     </row>
     <row r="39" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B39" s="1"/>
       <c r="C39" s="3">
         <v>622</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E39" s="1"/>
       <c r="F39" s="3">
@@ -2115,10 +2115,10 @@
     </row>
     <row r="40" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="C40" s="3">
         <v>529</v>
@@ -2154,10 +2154,10 @@
     </row>
     <row r="41" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" s="1" t="s">
-        <v>76</v>
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="3">
@@ -2180,7 +2180,7 @@
         <v>608</v>
       </c>
       <c r="K41" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="L41" s="3">
         <v>509</v>
@@ -2195,14 +2195,14 @@
     </row>
     <row r="42" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B42" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="E42" s="1"/>
       <c r="F42" s="3">
@@ -2232,7 +2232,7 @@
     </row>
     <row r="43" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B43" s="1"/>
       <c r="C43" s="1"/>
@@ -2261,7 +2261,7 @@
     </row>
     <row r="44" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B44" s="1"/>
       <c r="C44" s="1"/>
@@ -2294,11 +2294,11 @@
     </row>
     <row r="45" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B45" s="1"/>
       <c r="C45" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D45" s="3">
         <v>501</v>
@@ -2333,7 +2333,7 @@
     </row>
     <row r="46" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B46" s="1"/>
       <c r="C46" s="1"/>
@@ -2362,7 +2362,7 @@
     </row>
     <row r="47" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B47" s="1"/>
       <c r="C47" s="1"/>
@@ -2399,10 +2399,10 @@
     </row>
     <row r="48" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B48" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C48" s="3">
         <v>605</v>
@@ -2423,7 +2423,7 @@
         <v>605</v>
       </c>
       <c r="K48" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="L48" s="1"/>
       <c r="M48" s="1"/>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="49" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B49" s="1"/>
       <c r="C49" s="1"/>
@@ -2444,10 +2444,10 @@
         <v>512</v>
       </c>
       <c r="E49" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F49" s="1" t="s">
         <v>91</v>
-      </c>
-      <c r="F49" s="1" t="s">
-        <v>92</v>
       </c>
       <c r="G49" s="3">
         <v>606</v>
@@ -2475,10 +2475,10 @@
     </row>
     <row r="50" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B50" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="B50" s="1" t="s">
-        <v>94</v>
       </c>
       <c r="C50" s="3">
         <v>526</v>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="51" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B51" s="1"/>
       <c r="C51" s="3">
@@ -2536,7 +2536,7 @@
       </c>
       <c r="J51" s="1"/>
       <c r="K51" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="L51" s="1"/>
       <c r="M51" s="1"/>
@@ -2547,7 +2547,7 @@
     </row>
     <row r="52" spans="1:15" ht="12.75" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B52" s="1"/>
       <c r="C52" s="3">

</xml_diff>